<commit_message>
rebuilt the app structure
</commit_message>
<xml_diff>
--- a/analytics.xlsx
+++ b/analytics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Downloads\EY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798BDC3A-269E-4F1C-BA76-D53B2B67C403}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A17B62-8330-429F-BA94-36FA227BB82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2008" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="197">
   <si>
     <t>Date</t>
   </si>
@@ -1374,6 +1374,9 @@
       <t xml:space="preserve"> upcoming holidays.</t>
     </r>
   </si>
+  <si>
+    <t>Expiry</t>
+  </si>
 </sst>
 </file>
 
@@ -1734,10 +1737,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1746,7 +1749,7 @@
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" customHeight="1">
+    <row r="1" spans="1:13" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1783,8 +1786,11 @@
       <c r="L1" s="3" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M1" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1816,14 +1822,17 @@
         <v>0.41463414599999998</v>
       </c>
       <c r="K2">
-        <f ca="1">_xlfn.CEILING.MATH(J2+8*RAND())</f>
-        <v>2</v>
+        <f t="shared" ref="K2:K22" ca="1" si="0">_xlfn.CEILING.MATH(J2+8*RAND())</f>
+        <v>7</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1855,14 +1864,17 @@
         <v>0.86153846199999995</v>
       </c>
       <c r="K3">
-        <f ca="1">_xlfn.CEILING.MATH(J3+8*RAND())</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1894,14 +1906,17 @@
         <v>0.42499999999999999</v>
       </c>
       <c r="K4">
-        <f ca="1">_xlfn.CEILING.MATH(J4+8*RAND())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1933,14 +1948,17 @@
         <v>0.43333333299999999</v>
       </c>
       <c r="K5">
-        <f ca="1">_xlfn.CEILING.MATH(J5+8*RAND())</f>
-        <v>1</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1972,14 +1990,17 @@
         <v>0.8</v>
       </c>
       <c r="K6">
-        <f ca="1">_xlfn.CEILING.MATH(J6+8*RAND())</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M6">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2011,14 +2032,17 @@
         <v>1.2</v>
       </c>
       <c r="K7">
-        <f ca="1">_xlfn.CEILING.MATH(J7+8*RAND())</f>
-        <v>4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M7">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2050,14 +2074,17 @@
         <v>2.2588235289999998</v>
       </c>
       <c r="K8">
-        <f ca="1">_xlfn.CEILING.MATH(J8+8*RAND())</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M8">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -2089,14 +2116,17 @@
         <v>0.34482758600000002</v>
       </c>
       <c r="K9">
-        <f ca="1">_xlfn.CEILING.MATH(J9+8*RAND())</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2128,14 +2158,17 @@
         <v>0.35466666699999999</v>
       </c>
       <c r="K10">
-        <f ca="1">_xlfn.CEILING.MATH(J10+8*RAND())</f>
-        <v>8</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2167,14 +2200,17 @@
         <v>1.081081081</v>
       </c>
       <c r="K11">
-        <f ca="1">_xlfn.CEILING.MATH(J11+8*RAND())</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M11">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2206,14 +2242,17 @@
         <v>1.636363636</v>
       </c>
       <c r="K12">
-        <f ca="1">_xlfn.CEILING.MATH(J12+8*RAND())</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2245,14 +2284,17 @@
         <v>0.51282051299999998</v>
       </c>
       <c r="K13">
-        <f ca="1">_xlfn.CEILING.MATH(J13+8*RAND())</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M13">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2284,14 +2326,17 @@
         <v>0.6</v>
       </c>
       <c r="K14">
-        <f ca="1">_xlfn.CEILING.MATH(J14+8*RAND())</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>189</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -2323,14 +2368,17 @@
         <v>0.5</v>
       </c>
       <c r="K15">
-        <f ca="1">_xlfn.CEILING.MATH(J15+8*RAND())</f>
-        <v>3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -2362,14 +2410,17 @@
         <v>1.6</v>
       </c>
       <c r="K16">
-        <f ca="1">_xlfn.CEILING.MATH(J16+8*RAND())</f>
-        <v>8</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>10</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M16">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2401,14 +2452,17 @@
         <v>1.52</v>
       </c>
       <c r="K17">
-        <f ca="1">_xlfn.CEILING.MATH(J17+8*RAND())</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -2440,14 +2494,17 @@
         <v>0.64800000000000002</v>
       </c>
       <c r="K18">
-        <f ca="1">_xlfn.CEILING.MATH(J18+8*RAND())</f>
-        <v>2</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" ht="15.75" customHeight="1">
+      <c r="M18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -2479,14 +2536,17 @@
         <v>1.6628571430000001</v>
       </c>
       <c r="K19">
-        <f ca="1">_xlfn.CEILING.MATH(J19+8*RAND())</f>
-        <v>6</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
       </c>
       <c r="L19" s="10" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="12.5">
+      <c r="M19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="12.5">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -2518,14 +2578,17 @@
         <v>2.5</v>
       </c>
       <c r="K20">
-        <f ca="1">_xlfn.CEILING.MATH(J20+8*RAND())</f>
-        <v>7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" ht="12.5">
+      <c r="M20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="12.5">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -2557,11 +2620,14 @@
         <v>3.62</v>
       </c>
       <c r="K21">
-        <f ca="1">_xlfn.CEILING.MATH(J21+8*RAND())</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="12.5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M21">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="12.5">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -2593,8 +2659,11 @@
         <v>2.7857142860000002</v>
       </c>
       <c r="K22">
-        <f ca="1">_xlfn.CEILING.MATH(J22+8*RAND())</f>
-        <v>5</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="M22">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -62257,7 +62326,7 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D8" ca="1" si="1">ROUNDUP(RANDBETWEEN(10, 30) * 10, 0)</f>
-        <v>220</v>
+        <v>190</v>
       </c>
       <c r="E2" s="3">
         <v>290</v>
@@ -62287,7 +62356,7 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="E3" s="3">
         <v>125</v>
@@ -62317,7 +62386,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>140</v>
+        <v>100</v>
       </c>
       <c r="E4" s="3">
         <v>85</v>
@@ -62347,7 +62416,7 @@
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>120</v>
+        <v>150</v>
       </c>
       <c r="E5" s="3">
         <v>150</v>
@@ -62377,7 +62446,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>240</v>
+        <v>100</v>
       </c>
       <c r="E6" s="3">
         <v>300</v>
@@ -62407,7 +62476,7 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>280</v>
       </c>
       <c r="E7" s="3">
         <v>390</v>
@@ -62437,7 +62506,7 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>290</v>
+        <v>190</v>
       </c>
       <c r="E8" s="3">
         <v>410</v>
@@ -62467,7 +62536,7 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" ref="D9:D15" ca="1" si="4">RANDBETWEEN(100,300)</f>
-        <v>242</v>
+        <v>129</v>
       </c>
       <c r="E9" s="3">
         <v>50</v>
@@ -62497,7 +62566,7 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="E10" s="3">
         <v>175</v>
@@ -62527,7 +62596,7 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>295</v>
+        <v>125</v>
       </c>
       <c r="E11" s="3">
         <v>375</v>
@@ -62557,7 +62626,7 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>234</v>
+        <v>180</v>
       </c>
       <c r="E12" s="3">
         <v>70</v>
@@ -62587,7 +62656,7 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E13" s="3">
         <v>210</v>
@@ -62617,7 +62686,7 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>195</v>
+        <v>297</v>
       </c>
       <c r="E14" s="3">
         <v>250</v>
@@ -62647,7 +62716,7 @@
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>135</v>
+        <v>181</v>
       </c>
       <c r="E15" s="3">
         <v>90</v>
@@ -62677,7 +62746,7 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" ref="D16:D22" ca="1" si="5">ROUNDUP(RANDBETWEEN(10, 30) * 10, 0)</f>
-        <v>260</v>
+        <v>300</v>
       </c>
       <c r="E16" s="3">
         <v>500</v>
@@ -62707,7 +62776,7 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="E17" s="3">
         <v>325</v>
@@ -62737,7 +62806,7 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="E18" s="3">
         <v>185</v>
@@ -62767,7 +62836,7 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>160</v>
+        <v>250</v>
       </c>
       <c r="E19" s="3">
         <v>200</v>
@@ -62797,7 +62866,7 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>130</v>
+        <v>200</v>
       </c>
       <c r="E20" s="3">
         <v>75</v>
@@ -62827,7 +62896,7 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>270</v>
+        <v>210</v>
       </c>
       <c r="E21" s="3">
         <v>165</v>
@@ -62921,7 +62990,7 @@
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B22" ca="1" si="0">DATE(2023,10,INT(RAND()*15)+1)</f>
-        <v>45207</v>
+        <v>45212</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>Inventory!D2</f>
@@ -62936,7 +63005,7 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">D2+RANDBETWEEN(-8,8)</f>
-        <v>404</v>
+        <v>417</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
@@ -62946,7 +63015,7 @@
       </c>
       <c r="B3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45203</v>
+        <v>45200</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>Inventory!D3</f>
@@ -62961,7 +63030,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F22" ca="1" si="1">D3+RANDBETWEEN(-5,5)</f>
-        <v>322</v>
+        <v>323</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
@@ -62971,7 +63040,7 @@
       </c>
       <c r="B4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45203</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>Inventory!D4</f>
@@ -62986,7 +63055,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
@@ -62996,7 +63065,7 @@
       </c>
       <c r="B5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45204</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>Inventory!D5</f>
@@ -63011,7 +63080,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>305</v>
+        <v>301</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
@@ -63021,7 +63090,7 @@
       </c>
       <c r="B6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45201</v>
+        <v>45200</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>Inventory!D6</f>
@@ -63036,7 +63105,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
@@ -63046,7 +63115,7 @@
       </c>
       <c r="B7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45213</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>Inventory!D7</f>
@@ -63071,7 +63140,7 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45200</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>Inventory!D8</f>
@@ -63086,7 +63155,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
@@ -63096,7 +63165,7 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45201</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>Inventory!D9</f>
@@ -63111,7 +63180,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
@@ -63121,7 +63190,7 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45201</v>
+        <v>45205</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>Inventory!D10</f>
@@ -63136,7 +63205,7 @@
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1">
@@ -63146,7 +63215,7 @@
       </c>
       <c r="B11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45202</v>
+        <v>45213</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>Inventory!D11</f>
@@ -63161,7 +63230,7 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>185</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
@@ -63171,7 +63240,7 @@
       </c>
       <c r="B12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45206</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>Inventory!D12</f>
@@ -63196,7 +63265,7 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45211</v>
+        <v>45205</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>Inventory!D13</f>
@@ -63211,7 +63280,7 @@
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>395</v>
+        <v>386</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="15.75" customHeight="1">
@@ -63221,7 +63290,7 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45209</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>Inventory!D14</f>
@@ -63236,7 +63305,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>206</v>
+        <v>214</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
@@ -63246,7 +63315,7 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45211</v>
+        <v>45200</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>Inventory!D15</f>
@@ -63261,7 +63330,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>503</v>
+        <v>495</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
@@ -63271,7 +63340,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45214</v>
+        <v>45208</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>Inventory!D16</f>
@@ -63286,7 +63355,7 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
@@ -63296,7 +63365,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45214</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>Inventory!D17</f>
@@ -63311,7 +63380,7 @@
       </c>
       <c r="F17" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
@@ -63321,7 +63390,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45204</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>Inventory!D18</f>
@@ -63361,7 +63430,7 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.5">
@@ -63371,7 +63440,7 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45207</v>
+        <v>45213</v>
       </c>
       <c r="C20" s="7" t="str">
         <f>Inventory!D20</f>
@@ -63386,7 +63455,7 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.5">
@@ -63396,7 +63465,7 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45206</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>Inventory!D21</f>
@@ -63411,7 +63480,7 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.5">
@@ -63421,7 +63490,7 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45209</v>
+        <v>45213</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>Inventory!D22</f>
@@ -63436,7 +63505,7 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed text to speech function
</commit_message>
<xml_diff>
--- a/analytics.xlsx
+++ b/analytics.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kshit\Downloads\EY\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A17B62-8330-429F-BA94-36FA227BB82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1417D84C-56B8-4A33-823A-D3E735EF04DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2009" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2010" uniqueCount="198">
   <si>
     <t>Date</t>
   </si>
@@ -1377,12 +1377,15 @@
   <si>
     <t>Expiry</t>
   </si>
+  <si>
+    <t>Predicted Price after 15 days (%)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1451,6 +1454,12 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FF00A67D"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1484,7 +1493,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1502,6 +1511,9 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1737,19 +1749,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:M22"/>
+  <dimension ref="A1:R22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="15.6328125" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" customWidth="1"/>
+    <col min="14" max="14" width="12.6328125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" customHeight="1">
+    <row r="1" spans="1:18" ht="15.75" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -1789,8 +1802,12 @@
       <c r="M1" s="3" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N1" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="R1" s="11"/>
+    </row>
+    <row r="2" spans="1:18" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
@@ -1823,7 +1840,7 @@
       </c>
       <c r="K2">
         <f t="shared" ref="K2:K22" ca="1" si="0">_xlfn.CEILING.MATH(J2+8*RAND())</f>
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L2" s="10" t="s">
         <v>177</v>
@@ -1831,8 +1848,11 @@
       <c r="M2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N2" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -1865,7 +1885,7 @@
       </c>
       <c r="K3">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="L3" s="10" t="s">
         <v>178</v>
@@ -1873,8 +1893,11 @@
       <c r="M3">
         <v>45</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N3" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1907,7 +1930,7 @@
       </c>
       <c r="K4">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="L4" s="10" t="s">
         <v>179</v>
@@ -1915,8 +1938,11 @@
       <c r="M4">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N4" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1949,7 +1975,7 @@
       </c>
       <c r="K5">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="10" t="s">
         <v>180</v>
@@ -1957,8 +1983,11 @@
       <c r="M5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N5" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -1991,7 +2020,7 @@
       </c>
       <c r="K6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>181</v>
@@ -1999,8 +2028,11 @@
       <c r="M6">
         <v>45</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N6" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
@@ -2033,7 +2065,7 @@
       </c>
       <c r="K7">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>182</v>
@@ -2041,8 +2073,11 @@
       <c r="M7">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N7" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -2075,7 +2110,7 @@
       </c>
       <c r="K8">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L8" s="10" t="s">
         <v>183</v>
@@ -2083,8 +2118,11 @@
       <c r="M8">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N8" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -2117,7 +2155,7 @@
       </c>
       <c r="K9">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L9" s="10" t="s">
         <v>184</v>
@@ -2125,8 +2163,11 @@
       <c r="M9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N9" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>12</v>
       </c>
@@ -2159,7 +2200,7 @@
       </c>
       <c r="K10">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L10" s="10" t="s">
         <v>185</v>
@@ -2167,8 +2208,11 @@
       <c r="M10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N10" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -2201,7 +2245,7 @@
       </c>
       <c r="K11">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="L11" s="10" t="s">
         <v>186</v>
@@ -2209,8 +2253,11 @@
       <c r="M11">
         <v>25</v>
       </c>
-    </row>
-    <row r="12" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N11" s="12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2243,7 +2290,7 @@
       </c>
       <c r="K12">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L12" s="10" t="s">
         <v>187</v>
@@ -2251,8 +2298,11 @@
       <c r="M12">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N12" s="12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>14</v>
       </c>
@@ -2285,7 +2335,7 @@
       </c>
       <c r="K13">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L13" s="10" t="s">
         <v>188</v>
@@ -2293,8 +2343,11 @@
       <c r="M13">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N13" s="12">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -2327,7 +2380,7 @@
       </c>
       <c r="K14">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L14" s="10" t="s">
         <v>189</v>
@@ -2335,8 +2388,11 @@
       <c r="M14">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N14" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>10</v>
       </c>
@@ -2369,7 +2425,7 @@
       </c>
       <c r="K15">
         <f t="shared" ca="1" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L15" s="10" t="s">
         <v>190</v>
@@ -2377,8 +2433,11 @@
       <c r="M15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N15" s="12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -2411,7 +2470,7 @@
       </c>
       <c r="K16">
         <f t="shared" ca="1" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="L16" s="10" t="s">
         <v>191</v>
@@ -2419,8 +2478,11 @@
       <c r="M16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N16" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>14</v>
       </c>
@@ -2453,7 +2515,7 @@
       </c>
       <c r="K17">
         <f t="shared" ca="1" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="L17" s="10" t="s">
         <v>192</v>
@@ -2461,8 +2523,11 @@
       <c r="M17">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N17" s="12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
         <v>12</v>
       </c>
@@ -2495,7 +2560,7 @@
       </c>
       <c r="K18">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="L18" s="10" t="s">
         <v>193</v>
@@ -2503,8 +2568,11 @@
       <c r="M18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" ht="15.75" customHeight="1">
+      <c r="N18" s="12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
         <v>12</v>
       </c>
@@ -2545,8 +2613,11 @@
       <c r="M19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" ht="12.5">
+      <c r="N19" s="12">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="12.5">
       <c r="A20" s="3" t="s">
         <v>12</v>
       </c>
@@ -2579,7 +2650,7 @@
       </c>
       <c r="K20">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L20" s="10" t="s">
         <v>195</v>
@@ -2587,8 +2658,11 @@
       <c r="M20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" ht="12.5">
+      <c r="N20" s="12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="12.5">
       <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
@@ -2621,13 +2695,16 @@
       </c>
       <c r="K21">
         <f t="shared" ca="1" si="0"/>
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="M21">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" ht="12.5">
+      <c r="N21" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="12.5">
       <c r="A22" s="3" t="s">
         <v>12</v>
       </c>
@@ -2660,10 +2737,13 @@
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="0"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="M22">
         <v>15</v>
+      </c>
+      <c r="N22" s="12">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -62326,7 +62406,7 @@
       </c>
       <c r="D2" s="3">
         <f t="shared" ref="D2:D8" ca="1" si="1">ROUNDUP(RANDBETWEEN(10, 30) * 10, 0)</f>
-        <v>190</v>
+        <v>250</v>
       </c>
       <c r="E2" s="3">
         <v>290</v>
@@ -62356,7 +62436,7 @@
       </c>
       <c r="D3" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>200</v>
+        <v>140</v>
       </c>
       <c r="E3" s="3">
         <v>125</v>
@@ -62386,7 +62466,7 @@
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>180</v>
       </c>
       <c r="E4" s="3">
         <v>85</v>
@@ -62446,7 +62526,7 @@
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>100</v>
+        <v>210</v>
       </c>
       <c r="E6" s="3">
         <v>300</v>
@@ -62476,7 +62556,7 @@
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>280</v>
+        <v>110</v>
       </c>
       <c r="E7" s="3">
         <v>390</v>
@@ -62506,7 +62586,7 @@
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>190</v>
+        <v>130</v>
       </c>
       <c r="E8" s="3">
         <v>410</v>
@@ -62536,7 +62616,7 @@
       </c>
       <c r="D9" s="3">
         <f t="shared" ref="D9:D15" ca="1" si="4">RANDBETWEEN(100,300)</f>
-        <v>129</v>
+        <v>198</v>
       </c>
       <c r="E9" s="3">
         <v>50</v>
@@ -62566,7 +62646,7 @@
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>236</v>
+        <v>295</v>
       </c>
       <c r="E10" s="3">
         <v>175</v>
@@ -62596,7 +62676,7 @@
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>125</v>
+        <v>244</v>
       </c>
       <c r="E11" s="3">
         <v>375</v>
@@ -62626,7 +62706,7 @@
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="E12" s="3">
         <v>70</v>
@@ -62656,7 +62736,7 @@
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>106</v>
+        <v>261</v>
       </c>
       <c r="E13" s="3">
         <v>210</v>
@@ -62686,7 +62766,7 @@
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="4"/>
-        <v>297</v>
+        <v>192</v>
       </c>
       <c r="E14" s="3">
         <v>250</v>
@@ -62746,7 +62826,7 @@
       </c>
       <c r="D16" s="3">
         <f t="shared" ref="D16:D22" ca="1" si="5">ROUNDUP(RANDBETWEEN(10, 30) * 10, 0)</f>
-        <v>300</v>
+        <v>250</v>
       </c>
       <c r="E16" s="3">
         <v>500</v>
@@ -62776,7 +62856,7 @@
       </c>
       <c r="D17" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>220</v>
+        <v>200</v>
       </c>
       <c r="E17" s="3">
         <v>325</v>
@@ -62806,7 +62886,7 @@
       </c>
       <c r="D18" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>140</v>
+        <v>190</v>
       </c>
       <c r="E18" s="3">
         <v>185</v>
@@ -62836,7 +62916,7 @@
       </c>
       <c r="D19" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>250</v>
+        <v>200</v>
       </c>
       <c r="E19" s="3">
         <v>200</v>
@@ -62866,7 +62946,7 @@
       </c>
       <c r="D20" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>200</v>
+        <v>230</v>
       </c>
       <c r="E20" s="3">
         <v>75</v>
@@ -62896,7 +62976,7 @@
       </c>
       <c r="D21" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>210</v>
+        <v>260</v>
       </c>
       <c r="E21" s="3">
         <v>165</v>
@@ -62926,7 +63006,7 @@
       </c>
       <c r="D22" s="3">
         <f t="shared" ca="1" si="5"/>
-        <v>280</v>
+        <v>210</v>
       </c>
       <c r="E22" s="3">
         <v>400</v>
@@ -62990,7 +63070,7 @@
       </c>
       <c r="B2" s="4">
         <f t="shared" ref="B2:B22" ca="1" si="0">DATE(2023,10,INT(RAND()*15)+1)</f>
-        <v>45212</v>
+        <v>45206</v>
       </c>
       <c r="C2" s="7" t="str">
         <f>Inventory!D2</f>
@@ -63005,7 +63085,7 @@
       </c>
       <c r="F2" s="3">
         <f ca="1">D2+RANDBETWEEN(-8,8)</f>
-        <v>417</v>
+        <v>418</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1">
@@ -63015,7 +63095,7 @@
       </c>
       <c r="B3" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45203</v>
       </c>
       <c r="C3" s="7" t="str">
         <f>Inventory!D3</f>
@@ -63030,7 +63110,7 @@
       </c>
       <c r="F3" s="3">
         <f t="shared" ref="F3:F22" ca="1" si="1">D3+RANDBETWEEN(-5,5)</f>
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1">
@@ -63040,7 +63120,7 @@
       </c>
       <c r="B4" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45203</v>
+        <v>45211</v>
       </c>
       <c r="C4" s="7" t="str">
         <f>Inventory!D4</f>
@@ -63055,7 +63135,7 @@
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>397</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1">
@@ -63065,7 +63145,7 @@
       </c>
       <c r="B5" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45209</v>
       </c>
       <c r="C5" s="7" t="str">
         <f>Inventory!D5</f>
@@ -63080,7 +63160,7 @@
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>301</v>
+        <v>304</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1">
@@ -63090,7 +63170,7 @@
       </c>
       <c r="B6" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45203</v>
       </c>
       <c r="C6" s="7" t="str">
         <f>Inventory!D6</f>
@@ -63105,7 +63185,7 @@
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>199</v>
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1">
@@ -63115,7 +63195,7 @@
       </c>
       <c r="B7" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45207</v>
       </c>
       <c r="C7" s="7" t="str">
         <f>Inventory!D7</f>
@@ -63130,7 +63210,7 @@
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>146</v>
+        <v>153</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1">
@@ -63140,7 +63220,7 @@
       </c>
       <c r="B8" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45212</v>
       </c>
       <c r="C8" s="7" t="str">
         <f>Inventory!D8</f>
@@ -63155,7 +63235,7 @@
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>85</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1">
@@ -63165,7 +63245,7 @@
       </c>
       <c r="B9" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45201</v>
+        <v>45203</v>
       </c>
       <c r="C9" s="7" t="str">
         <f>Inventory!D9</f>
@@ -63180,7 +63260,7 @@
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>287</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1">
@@ -63190,7 +63270,7 @@
       </c>
       <c r="B10" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45205</v>
+        <v>45211</v>
       </c>
       <c r="C10" s="7" t="str">
         <f>Inventory!D10</f>
@@ -63215,7 +63295,7 @@
       </c>
       <c r="B11" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45204</v>
       </c>
       <c r="C11" s="7" t="str">
         <f>Inventory!D11</f>
@@ -63230,7 +63310,7 @@
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>188</v>
+        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" customHeight="1">
@@ -63240,7 +63320,7 @@
       </c>
       <c r="B12" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45204</v>
       </c>
       <c r="C12" s="7" t="str">
         <f>Inventory!D12</f>
@@ -63255,7 +63335,7 @@
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>163</v>
+        <v>167</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="15.75" customHeight="1">
@@ -63265,7 +63345,7 @@
       </c>
       <c r="B13" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45205</v>
+        <v>45214</v>
       </c>
       <c r="C13" s="7" t="str">
         <f>Inventory!D13</f>
@@ -63290,7 +63370,7 @@
       </c>
       <c r="B14" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45209</v>
+        <v>45200</v>
       </c>
       <c r="C14" s="7" t="str">
         <f>Inventory!D14</f>
@@ -63305,7 +63385,7 @@
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>214</v>
+        <v>208</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1">
@@ -63315,7 +63395,7 @@
       </c>
       <c r="B15" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45200</v>
+        <v>45207</v>
       </c>
       <c r="C15" s="7" t="str">
         <f>Inventory!D15</f>
@@ -63330,7 +63410,7 @@
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>495</v>
+        <v>503</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1">
@@ -63340,7 +63420,7 @@
       </c>
       <c r="B16" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45208</v>
+        <v>45207</v>
       </c>
       <c r="C16" s="7" t="str">
         <f>Inventory!D16</f>
@@ -63355,7 +63435,7 @@
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>78</v>
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
@@ -63365,7 +63445,7 @@
       </c>
       <c r="B17" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45214</v>
+        <v>45211</v>
       </c>
       <c r="C17" s="7" t="str">
         <f>Inventory!D17</f>
@@ -63390,7 +63470,7 @@
       </c>
       <c r="B18" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45204</v>
+        <v>45214</v>
       </c>
       <c r="C18" s="7" t="str">
         <f>Inventory!D18</f>
@@ -63405,7 +63485,7 @@
       </c>
       <c r="F18" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>246</v>
+        <v>254</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
@@ -63415,7 +63495,7 @@
       </c>
       <c r="B19" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45210</v>
       </c>
       <c r="C19" s="7" t="str">
         <f>Inventory!D19</f>
@@ -63430,7 +63510,7 @@
       </c>
       <c r="F19" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>173</v>
+        <v>175</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="12.5">
@@ -63440,7 +63520,7 @@
       </c>
       <c r="B20" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45203</v>
       </c>
       <c r="C20" s="7" t="str">
         <f>Inventory!D20</f>
@@ -63455,7 +63535,7 @@
       </c>
       <c r="F20" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="12.5">
@@ -63465,7 +63545,7 @@
       </c>
       <c r="B21" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45206</v>
+        <v>45207</v>
       </c>
       <c r="C21" s="7" t="str">
         <f>Inventory!D21</f>
@@ -63480,7 +63560,7 @@
       </c>
       <c r="F21" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="12.5">
@@ -63490,7 +63570,7 @@
       </c>
       <c r="B22" s="4">
         <f t="shared" ca="1" si="0"/>
-        <v>45213</v>
+        <v>45214</v>
       </c>
       <c r="C22" s="7" t="str">
         <f>Inventory!D22</f>
@@ -63505,7 +63585,7 @@
       </c>
       <c r="F22" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>